<commit_message>
TAC done, Kethane beginning.
</commit_message>
<xml_diff>
--- a/Source/CalcsAndModels/ModTanks.xlsx
+++ b/Source/CalcsAndModels/ModTanks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Mass</t>
   </si>
@@ -162,15 +162,6 @@
     <t>Kethane</t>
   </si>
   <si>
-    <t>tankk1mLarge</t>
-  </si>
-  <si>
-    <t>1m Large Tank</t>
-  </si>
-  <si>
-    <t>1m Standard Tank</t>
-  </si>
-  <si>
     <t>tank1mStandard</t>
   </si>
   <si>
@@ -193,6 +184,12 @@
   </si>
   <si>
     <t>tank2mMedium</t>
+  </si>
+  <si>
+    <t>tank2mSmall</t>
+  </si>
+  <si>
+    <t>KE-TM30</t>
   </si>
 </sst>
 </file>
@@ -547,7 +544,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -565,25 +562,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,7 +583,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1013,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1150,109 +1146,109 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16" thickBot="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="30"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="23"/>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>0.625</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>0.125</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>0.02</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="17">
+      <c r="F4" s="12"/>
+      <c r="G4" s="15">
         <v>30</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="14" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="12">
         <v>60</v>
       </c>
       <c r="L4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="11">
         <v>0.2</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="14">
         <v>0.2</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="12">
         <v>1</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="15">
         <v>12</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="11">
         <v>500</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="12">
         <v>500</v>
       </c>
-      <c r="S4" s="11">
+      <c r="S4" s="15">
         <v>3200</v>
       </c>
-      <c r="T4" s="12">
+      <c r="T4" s="11">
         <f>PI()*(0.5*C4)*(0.5*C4)*D4</f>
         <v>3.8349519697141031E-2</v>
       </c>
-      <c r="U4" s="15">
+      <c r="U4" s="14">
         <f>E4/$T4</f>
         <v>0.52151891752352264</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="14">
         <f>G4/$T4</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W4" s="13">
+      <c r="W4" s="12">
         <f>K4/$T4</f>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X4" s="15">
+      <c r="X4" s="14">
         <f>G4/E4</f>
         <v>1500</v>
       </c>
-      <c r="Y4" s="15">
+      <c r="Y4" s="14">
         <f>G4/E4</f>
         <v>1500</v>
       </c>
-      <c r="Z4" s="13">
+      <c r="Z4" s="12">
         <f>K4/E4</f>
         <v>3000</v>
       </c>
@@ -1261,76 +1257,76 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>1.25</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.25</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="17">
+      <c r="F5" s="12"/>
+      <c r="G5" s="15">
         <v>240</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="14" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="12">
         <v>480</v>
       </c>
       <c r="L5" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="11">
         <v>0.2</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="14">
         <v>0.2</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="12">
         <v>1</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="15">
         <v>12</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="11">
         <v>500</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="12">
         <v>500</v>
       </c>
-      <c r="S5" s="11">
+      <c r="S5" s="15">
         <v>3200</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="11">
         <f t="shared" ref="T5:T21" si="0">PI()*(0.5*C5)*(0.5*C5)*D5</f>
         <v>0.30679615757712825</v>
       </c>
-      <c r="U5" s="15">
+      <c r="U5" s="14">
         <f t="shared" ref="U5:U21" si="1">E5/$T5</f>
         <v>0.22816452641654117</v>
       </c>
-      <c r="V5" s="15">
+      <c r="V5" s="14">
         <f t="shared" ref="V5:V6" si="2">G5/$T5</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W5" s="13">
+      <c r="W5" s="12">
         <f t="shared" ref="W5:W15" si="3">K5/$T5</f>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X5" s="15">
-        <f t="shared" ref="X5:Y6" si="4">G5/E5</f>
+      <c r="X5" s="14">
+        <f t="shared" ref="X5:X6" si="4">G5/E5</f>
         <v>3428.5714285714284</v>
       </c>
-      <c r="Y5" s="15">
+      <c r="Y5" s="14">
         <f t="shared" ref="Y5:Y6" si="5">G5/E5</f>
         <v>3428.5714285714284</v>
       </c>
-      <c r="Z5" s="13">
+      <c r="Z5" s="12">
         <f t="shared" ref="Z5:Z6" si="6">K5/E5</f>
         <v>6857.1428571428569</v>
       </c>
@@ -1339,78 +1335,78 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>2.5</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>0.5</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>0.15</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="12">
         <v>0.15</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="15">
         <v>1920</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="14" t="s">
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="12">
         <v>3840</v>
       </c>
       <c r="L6" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="11">
         <v>0.2</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="14">
         <v>0.2</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="12">
         <v>1</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="15">
         <v>12</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="11">
         <v>500</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="12">
         <v>500</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S6" s="15">
         <v>3200</v>
       </c>
-      <c r="T6" s="12">
+      <c r="T6" s="11">
         <f t="shared" si="0"/>
         <v>2.454369260617026</v>
       </c>
-      <c r="U6" s="15">
+      <c r="U6" s="14">
         <f t="shared" si="1"/>
         <v>6.1115498147287804E-2</v>
       </c>
-      <c r="V6" s="15">
+      <c r="V6" s="14">
         <f t="shared" si="2"/>
         <v>782.27837628528391</v>
       </c>
-      <c r="W6" s="13">
+      <c r="W6" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X6" s="15">
+      <c r="X6" s="14">
         <f t="shared" si="4"/>
         <v>12800</v>
       </c>
-      <c r="Y6" s="15">
+      <c r="Y6" s="14">
         <f t="shared" si="5"/>
         <v>12800</v>
       </c>
-      <c r="Z6" s="13">
+      <c r="Z6" s="12">
         <f t="shared" si="6"/>
         <v>25600</v>
       </c>
@@ -1419,74 +1415,74 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>0.625</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>0.125</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>0.02</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="17">
+      <c r="F7" s="12"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15">
         <v>30</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="14" t="s">
+      <c r="I7" s="15"/>
+      <c r="J7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="12">
         <v>60</v>
       </c>
       <c r="L7" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="11">
         <v>0.2</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="14">
         <v>0.2</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="12">
         <v>1</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="15">
         <v>12</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="11">
         <v>500</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="12">
         <v>500</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="15">
         <v>3200</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="11">
         <f t="shared" si="0"/>
         <v>3.8349519697141031E-2</v>
       </c>
-      <c r="U7" s="15">
+      <c r="U7" s="14">
         <f t="shared" si="1"/>
         <v>0.52151891752352264</v>
       </c>
-      <c r="V7" s="15">
+      <c r="V7" s="14">
         <f>H7/$T7</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W7" s="13">
+      <c r="W7" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X7" s="15">
+      <c r="X7" s="14">
         <v>1500</v>
       </c>
-      <c r="Y7" s="15">
+      <c r="Y7" s="14">
         <v>1500</v>
       </c>
-      <c r="Z7" s="13">
+      <c r="Z7" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -1494,74 +1490,74 @@
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>1.25</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>0.25</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="17">
+      <c r="F8" s="12"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15">
         <v>240</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="14" t="s">
+      <c r="I8" s="15"/>
+      <c r="J8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="12">
         <v>480</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="11">
         <v>0.2</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="14">
         <v>0.2</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="12">
         <v>1</v>
       </c>
-      <c r="P8" s="11">
+      <c r="P8" s="15">
         <v>12</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="11">
         <v>500</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="12">
         <v>500</v>
       </c>
-      <c r="S8" s="11">
+      <c r="S8" s="15">
         <v>3200</v>
       </c>
-      <c r="T8" s="12">
+      <c r="T8" s="11">
         <f t="shared" si="0"/>
         <v>0.30679615757712825</v>
       </c>
-      <c r="U8" s="15">
+      <c r="U8" s="14">
         <f t="shared" si="1"/>
         <v>0.22816452641654117</v>
       </c>
-      <c r="V8" s="15">
+      <c r="V8" s="14">
         <f t="shared" ref="V8:V9" si="7">H8/$T8</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W8" s="13">
+      <c r="W8" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X8" s="15">
+      <c r="X8" s="14">
         <v>3428.57143</v>
       </c>
-      <c r="Y8" s="15">
+      <c r="Y8" s="14">
         <v>3428.57143</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="Z8" s="12">
         <v>6857.14</v>
       </c>
     </row>
@@ -1569,74 +1565,74 @@
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>2.5</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>0.5</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0.15</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="17">
+      <c r="F9" s="12"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15">
         <v>1920</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="14" t="s">
+      <c r="I9" s="15"/>
+      <c r="J9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="12">
         <v>3840</v>
       </c>
       <c r="L9" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="11">
         <v>0.2</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="14">
         <v>0.2</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="12">
         <v>1</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="15">
         <v>12</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="11">
         <v>500</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="12">
         <v>500</v>
       </c>
-      <c r="S9" s="11">
+      <c r="S9" s="15">
         <v>3200</v>
       </c>
-      <c r="T9" s="12">
+      <c r="T9" s="11">
         <f t="shared" si="0"/>
         <v>2.454369260617026</v>
       </c>
-      <c r="U9" s="15">
+      <c r="U9" s="14">
         <f t="shared" si="1"/>
         <v>6.1115498147287804E-2</v>
       </c>
-      <c r="V9" s="15">
+      <c r="V9" s="14">
         <f t="shared" si="7"/>
         <v>782.27837628528391</v>
       </c>
-      <c r="W9" s="13">
+      <c r="W9" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X9" s="15">
+      <c r="X9" s="14">
         <v>12800</v>
       </c>
-      <c r="Y9" s="15">
+      <c r="Y9" s="14">
         <v>12800</v>
       </c>
-      <c r="Z9" s="13">
+      <c r="Z9" s="12">
         <v>25600</v>
       </c>
     </row>
@@ -1644,74 +1640,74 @@
       <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>0.625</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <v>0.125</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>0.02</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17">
+      <c r="F10" s="12"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15">
         <v>30</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="12">
         <v>60</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="11">
         <v>0.2</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="14">
         <v>0.2</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="12">
         <v>1</v>
       </c>
-      <c r="P10" s="11">
+      <c r="P10" s="15">
         <v>12</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="11">
         <v>500</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="12">
         <v>500</v>
       </c>
-      <c r="S10" s="11">
+      <c r="S10" s="15">
         <v>3200</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10" s="11">
         <f t="shared" si="0"/>
         <v>3.8349519697141031E-2</v>
       </c>
-      <c r="U10" s="15">
+      <c r="U10" s="14">
         <f t="shared" si="1"/>
         <v>0.52151891752352264</v>
       </c>
-      <c r="V10" s="15">
+      <c r="V10" s="14">
         <f>I10/$T10</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W10" s="13">
+      <c r="W10" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X10" s="15">
+      <c r="X10" s="14">
         <v>1500</v>
       </c>
-      <c r="Y10" s="15">
+      <c r="Y10" s="14">
         <v>1500</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="Z10" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -1719,74 +1715,74 @@
       <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>1.25</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <v>0.25</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17">
+      <c r="F11" s="12"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15">
         <v>240</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="12">
         <v>480</v>
       </c>
       <c r="L11" t="s">
         <v>27</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="11">
         <v>0.2</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="14">
         <v>0.2</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="12">
         <v>1</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="15">
         <v>12</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="Q11" s="11">
         <v>500</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R11" s="12">
         <v>500</v>
       </c>
-      <c r="S11" s="11">
+      <c r="S11" s="15">
         <v>3200</v>
       </c>
-      <c r="T11" s="12">
+      <c r="T11" s="11">
         <f t="shared" si="0"/>
         <v>0.30679615757712825</v>
       </c>
-      <c r="U11" s="15">
+      <c r="U11" s="14">
         <f t="shared" si="1"/>
         <v>0.22816452641654117</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="14">
         <f t="shared" ref="V11:V12" si="8">I11/$T11</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W11" s="13">
+      <c r="W11" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X11" s="15">
+      <c r="X11" s="14">
         <v>3428.57143</v>
       </c>
-      <c r="Y11" s="15">
+      <c r="Y11" s="14">
         <v>3428.57143</v>
       </c>
-      <c r="Z11" s="13">
+      <c r="Z11" s="12">
         <v>6857.14</v>
       </c>
     </row>
@@ -1794,74 +1790,74 @@
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>2.5</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>0.5</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>0.15</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17">
+      <c r="F12" s="12"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
         <v>1920</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="12">
         <v>3840</v>
       </c>
       <c r="L12" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="11">
         <v>0.2</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="14">
         <v>0.2</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="12">
         <v>1</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P12" s="15">
         <v>12</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="11">
         <v>500</v>
       </c>
-      <c r="R12" s="10">
+      <c r="R12" s="12">
         <v>500</v>
       </c>
-      <c r="S12" s="11">
+      <c r="S12" s="15">
         <v>3200</v>
       </c>
-      <c r="T12" s="12">
+      <c r="T12" s="11">
         <f t="shared" si="0"/>
         <v>2.454369260617026</v>
       </c>
-      <c r="U12" s="15">
+      <c r="U12" s="14">
         <f t="shared" si="1"/>
         <v>6.1115498147287804E-2</v>
       </c>
-      <c r="V12" s="15">
+      <c r="V12" s="14">
         <f t="shared" si="8"/>
         <v>782.27837628528391</v>
       </c>
-      <c r="W12" s="13">
+      <c r="W12" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X12" s="15">
+      <c r="X12" s="14">
         <v>12800</v>
       </c>
-      <c r="Y12" s="15">
+      <c r="Y12" s="14">
         <v>12800</v>
       </c>
-      <c r="Z12" s="13">
+      <c r="Z12" s="12">
         <v>25600</v>
       </c>
     </row>
@@ -1869,78 +1865,78 @@
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>0.625</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <v>0.125</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>0.02</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="17">
+      <c r="F13" s="12"/>
+      <c r="G13" s="15">
         <v>10</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="15">
         <v>10</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="15">
         <v>10</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="12">
         <v>60</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="11">
         <v>0.2</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="14">
         <v>0.2</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="12">
         <v>1</v>
       </c>
-      <c r="P13" s="11">
+      <c r="P13" s="15">
         <v>12</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="11">
         <v>500</v>
       </c>
-      <c r="R13" s="10">
+      <c r="R13" s="12">
         <v>500</v>
       </c>
-      <c r="S13" s="11">
+      <c r="S13" s="15">
         <v>3200</v>
       </c>
-      <c r="T13" s="12">
+      <c r="T13" s="11">
         <f t="shared" si="0"/>
         <v>3.8349519697141031E-2</v>
       </c>
-      <c r="U13" s="15">
+      <c r="U13" s="14">
         <f t="shared" si="1"/>
         <v>0.52151891752352264</v>
       </c>
-      <c r="V13" s="15">
+      <c r="V13" s="14">
         <f>(G13+H13+I13)/$T13</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W13" s="13">
+      <c r="W13" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X13" s="15">
+      <c r="X13" s="14">
         <v>1500</v>
       </c>
-      <c r="Y13" s="15">
+      <c r="Y13" s="14">
         <v>1500</v>
       </c>
-      <c r="Z13" s="13">
+      <c r="Z13" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -1948,78 +1944,78 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>1.25</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <v>0.25</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="17">
+      <c r="F14" s="12"/>
+      <c r="G14" s="15">
         <v>80</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="15">
         <v>80</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="15">
         <v>80</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="12">
         <v>480</v>
       </c>
       <c r="L14" t="s">
         <v>27</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="11">
         <v>0.2</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="14">
         <v>0.2</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="12">
         <v>1</v>
       </c>
-      <c r="P14" s="11">
+      <c r="P14" s="15">
         <v>12</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="Q14" s="11">
         <v>500</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="12">
         <v>500</v>
       </c>
-      <c r="S14" s="11">
+      <c r="S14" s="15">
         <v>3200</v>
       </c>
-      <c r="T14" s="12">
+      <c r="T14" s="11">
         <f t="shared" si="0"/>
         <v>0.30679615757712825</v>
       </c>
-      <c r="U14" s="15">
+      <c r="U14" s="14">
         <f t="shared" si="1"/>
         <v>0.22816452641654117</v>
       </c>
-      <c r="V14" s="15">
-        <f t="shared" ref="V14:V21" si="9">(G14+H14+I14)/$T14</f>
+      <c r="V14" s="14">
+        <f t="shared" ref="V14:V15" si="9">(G14+H14+I14)/$T14</f>
         <v>782.27837628528391</v>
       </c>
-      <c r="W14" s="13">
+      <c r="W14" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X14" s="15">
+      <c r="X14" s="14">
         <v>3428.57143</v>
       </c>
-      <c r="Y14" s="15">
+      <c r="Y14" s="14">
         <v>3428.57143</v>
       </c>
-      <c r="Z14" s="13">
+      <c r="Z14" s="12">
         <v>6857.14</v>
       </c>
     </row>
@@ -2027,527 +2023,508 @@
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>2.5</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="12">
         <v>0.5</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>0.15</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="17">
+      <c r="F15" s="12"/>
+      <c r="G15" s="15">
         <v>640</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="15">
         <v>640</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="15">
         <v>640</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="12">
         <v>3840</v>
       </c>
       <c r="L15" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="11">
         <v>0.2</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="14">
         <v>0.2</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="12">
         <v>1</v>
       </c>
-      <c r="P15" s="11">
+      <c r="P15" s="15">
         <v>12</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="Q15" s="11">
         <v>500</v>
       </c>
-      <c r="R15" s="10">
+      <c r="R15" s="12">
         <v>500</v>
       </c>
-      <c r="S15" s="11">
+      <c r="S15" s="15">
         <v>3200</v>
       </c>
-      <c r="T15" s="12">
+      <c r="T15" s="11">
         <f t="shared" si="0"/>
         <v>2.454369260617026</v>
       </c>
-      <c r="U15" s="15">
+      <c r="U15" s="14">
         <f t="shared" si="1"/>
         <v>6.1115498147287804E-2</v>
       </c>
-      <c r="V15" s="15">
+      <c r="V15" s="14">
         <f t="shared" si="9"/>
         <v>782.27837628528391</v>
       </c>
-      <c r="W15" s="13">
+      <c r="W15" s="12">
         <f t="shared" si="3"/>
         <v>1564.5567525705678</v>
       </c>
-      <c r="X15" s="15">
+      <c r="X15" s="14">
         <v>12800</v>
       </c>
-      <c r="Y15" s="15">
+      <c r="Y15" s="14">
         <v>12800</v>
       </c>
-      <c r="Z15" s="13">
+      <c r="Z15" s="12">
         <v>25600</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="16" thickBot="1">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="23"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="25"/>
       <c r="L16" s="24"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="25"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="29"/>
     </row>
     <row r="17" spans="1:26">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="11">
         <v>1.25</v>
       </c>
-      <c r="D17" s="10">
-        <v>1.51</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="D17" s="12">
+        <v>1.8620000000000001</v>
+      </c>
+      <c r="E17" s="14">
         <v>0.25</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="17">
+      <c r="F17" s="12"/>
+      <c r="G17" s="15">
         <v>0</v>
       </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
       <c r="J17">
         <v>1000</v>
       </c>
-      <c r="K17" s="10"/>
+      <c r="K17" s="12"/>
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17" s="11">
         <v>0.2</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="15">
         <v>0.3</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="12">
         <v>2</v>
       </c>
-      <c r="P17" s="11">
+      <c r="P17" s="15">
         <v>70</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="Q17" s="11">
         <v>50</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="12">
         <v>50</v>
       </c>
-      <c r="S17" s="11">
+      <c r="S17" s="15">
         <v>3000</v>
       </c>
-      <c r="T17" s="12">
+      <c r="T17" s="11">
         <f t="shared" si="0"/>
-        <v>1.8530487917658547</v>
-      </c>
-      <c r="U17" s="15">
+        <v>2.2850177816344512</v>
+      </c>
+      <c r="U17" s="14">
         <f t="shared" si="1"/>
-        <v>0.13491279944213644</v>
-      </c>
-      <c r="V17">
+        <v>0.10940833896757574</v>
+      </c>
+      <c r="V17" s="14">
         <v>0</v>
       </c>
-      <c r="W17" s="10">
+      <c r="W17" s="12">
         <f>J17/$T17</f>
-        <v>539.65119776854579</v>
-      </c>
-      <c r="X17" s="16">
+        <v>437.63335587030298</v>
+      </c>
+      <c r="X17" s="15">
         <v>0</v>
       </c>
-      <c r="Y17">
-        <f>J17/E17</f>
+      <c r="Y17" s="14">
+        <f t="shared" ref="Y17:Y21" si="10">J17/E17</f>
         <v>4000</v>
       </c>
-      <c r="Z17" s="10">
-        <f>J17/E17</f>
+      <c r="Z17" s="12">
+        <f t="shared" ref="Z17:Z21" si="11">J17/E17</f>
         <v>4000</v>
       </c>
     </row>
     <row r="18" spans="1:26">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="9">
-        <v>1.25</v>
-      </c>
-      <c r="D18" s="10">
-        <v>1.8620000000000001</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="17">
+      <c r="C18" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="D18" s="12">
+        <v>6.5784000000000002</v>
+      </c>
+      <c r="E18" s="14">
+        <v>3.25</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="15">
         <v>0</v>
       </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
       <c r="J18">
-        <v>1000</v>
-      </c>
-      <c r="K18" s="10"/>
+        <v>16000</v>
+      </c>
+      <c r="K18" s="12"/>
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="11">
         <v>0.2</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="15">
         <v>0.3</v>
       </c>
-      <c r="O18" s="10">
+      <c r="O18" s="12">
         <v>2</v>
       </c>
-      <c r="P18" s="11">
-        <v>70</v>
-      </c>
-      <c r="Q18" s="9">
-        <v>50</v>
-      </c>
-      <c r="R18" s="10">
-        <v>50</v>
-      </c>
-      <c r="S18" s="11">
-        <v>3000</v>
-      </c>
-      <c r="T18" s="12">
+      <c r="P18" s="15">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>200</v>
+      </c>
+      <c r="R18" s="12">
+        <v>200</v>
+      </c>
+      <c r="S18" s="15">
+        <v>2900</v>
+      </c>
+      <c r="T18" s="11">
         <f t="shared" si="0"/>
-        <v>2.2850177816344512</v>
-      </c>
-      <c r="U18" s="15">
+        <v>32.29164548808609</v>
+      </c>
+      <c r="U18" s="14">
         <f t="shared" si="1"/>
-        <v>0.10940833896757574</v>
-      </c>
-      <c r="V18">
+        <v>0.10064522729877851</v>
+      </c>
+      <c r="V18" s="14">
         <v>0</v>
       </c>
-      <c r="W18" s="10">
+      <c r="W18" s="12">
         <f>J18/$T18</f>
-        <v>437.63335587030298</v>
-      </c>
-      <c r="X18" s="16">
+        <v>495.48419593244807</v>
+      </c>
+      <c r="X18" s="15">
         <v>0</v>
       </c>
-      <c r="Y18">
-        <f t="shared" ref="Y18:Y21" si="10">J18/E18</f>
-        <v>4000</v>
-      </c>
-      <c r="Z18" s="10">
-        <f t="shared" ref="Z18:Z21" si="11">J18/E18</f>
-        <v>4000</v>
+      <c r="Y18" s="14">
+        <f>J18/E18</f>
+        <v>4923.0769230769229</v>
+      </c>
+      <c r="Z18" s="12">
+        <f>J18/E18</f>
+        <v>4923.0769230769229</v>
       </c>
     </row>
     <row r="19" spans="1:26">
       <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="9">
+      <c r="C19" s="11">
         <v>2.5</v>
       </c>
-      <c r="D19" s="10">
-        <v>6.5784000000000002</v>
-      </c>
-      <c r="E19" s="15">
-        <v>3.25</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="17">
+      <c r="D19" s="12">
+        <v>3.306</v>
+      </c>
+      <c r="E19" s="14">
+        <v>1.75</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="15">
         <v>0</v>
       </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
       <c r="J19">
-        <v>16000</v>
-      </c>
-      <c r="K19" s="10"/>
+        <v>8000</v>
+      </c>
+      <c r="K19" s="12"/>
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="11">
         <v>0.2</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="15">
         <v>0.3</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="12">
         <v>2</v>
       </c>
-      <c r="P19" s="11">
+      <c r="P19" s="15">
         <v>6</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="Q19" s="11">
         <v>200</v>
       </c>
-      <c r="R19" s="10">
+      <c r="R19" s="12">
         <v>200</v>
       </c>
-      <c r="S19" s="11">
+      <c r="S19" s="15">
         <v>2900</v>
       </c>
-      <c r="T19" s="12">
+      <c r="T19" s="11">
         <f t="shared" si="0"/>
-        <v>32.29164548808609</v>
-      </c>
-      <c r="U19" s="15">
+        <v>16.228289551199776</v>
+      </c>
+      <c r="U19" s="14">
         <f t="shared" si="1"/>
-        <v>0.10064522729877851</v>
-      </c>
-      <c r="V19">
+        <v>0.10783638007436344</v>
+      </c>
+      <c r="V19" s="14">
         <v>0</v>
       </c>
-      <c r="W19" s="10">
-        <f>J19/$T19</f>
-        <v>495.48419593244807</v>
-      </c>
-      <c r="X19" s="16">
+      <c r="W19" s="12">
+        <f t="shared" ref="W19:W21" si="12">J19/$T19</f>
+        <v>492.96630891137573</v>
+      </c>
+      <c r="X19" s="15">
         <v>0</v>
       </c>
-      <c r="Y19">
-        <f>J19/E19</f>
-        <v>4923.0769230769229</v>
-      </c>
-      <c r="Z19" s="10">
-        <f>J19/E19</f>
-        <v>4923.0769230769229</v>
+      <c r="Y19" s="14">
+        <f t="shared" si="10"/>
+        <v>4571.4285714285716</v>
+      </c>
+      <c r="Z19" s="12">
+        <f t="shared" si="11"/>
+        <v>4571.4285714285716</v>
       </c>
     </row>
     <row r="20" spans="1:26">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="11">
         <v>2.5</v>
       </c>
-      <c r="D20" s="10">
-        <v>3.306</v>
-      </c>
-      <c r="E20" s="15">
-        <v>1.75</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="17">
+      <c r="D20" s="12">
+        <v>1.8138000000000001</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="15">
         <v>0</v>
       </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="J20">
-        <v>8000</v>
-      </c>
-      <c r="K20" s="10"/>
+        <v>4000</v>
+      </c>
+      <c r="K20" s="12"/>
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="11">
         <v>0.2</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="15">
         <v>0.3</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="12">
         <v>2</v>
       </c>
-      <c r="P20" s="11">
+      <c r="P20" s="15">
         <v>6</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="Q20" s="11">
         <v>200</v>
       </c>
-      <c r="R20" s="10">
+      <c r="R20" s="12">
         <v>200</v>
       </c>
-      <c r="S20" s="11">
+      <c r="S20" s="15">
         <v>2900</v>
       </c>
-      <c r="T20" s="12">
+      <c r="T20" s="11">
         <f t="shared" si="0"/>
-        <v>16.228289551199776</v>
-      </c>
-      <c r="U20" s="15">
+        <v>8.9034699298143245</v>
+      </c>
+      <c r="U20" s="14">
         <f t="shared" si="1"/>
-        <v>0.10783638007436344</v>
-      </c>
-      <c r="V20">
+        <v>0.11231576092051274</v>
+      </c>
+      <c r="V20" s="14">
         <v>0</v>
       </c>
-      <c r="W20" s="10">
-        <f t="shared" ref="W18:W21" si="12">J20/$T20</f>
-        <v>492.96630891137573</v>
-      </c>
-      <c r="X20" s="16">
+      <c r="W20" s="12">
+        <f t="shared" si="12"/>
+        <v>449.26304368205098</v>
+      </c>
+      <c r="X20" s="15">
         <v>0</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" s="14">
         <f t="shared" si="10"/>
-        <v>4571.4285714285716</v>
-      </c>
-      <c r="Z20" s="10">
+        <v>4000</v>
+      </c>
+      <c r="Z20" s="12">
         <f t="shared" si="11"/>
-        <v>4571.4285714285716</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="21" spans="1:26">
       <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="9">
+      <c r="C21" s="11">
         <v>2.5</v>
       </c>
-      <c r="D21" s="10">
-        <v>1.8138000000000001</v>
-      </c>
-      <c r="E21" s="15">
-        <v>1</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="17">
+      <c r="D21" s="12">
+        <v>0.69120000000000004</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="15">
         <v>0</v>
       </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
       <c r="J21">
-        <v>4000</v>
-      </c>
-      <c r="K21" s="10"/>
+        <v>2000</v>
+      </c>
+      <c r="K21" s="12"/>
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="11">
         <v>0.2</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="15">
         <v>0.3</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="12">
         <v>2</v>
       </c>
-      <c r="P21" s="11">
+      <c r="P21" s="15">
         <v>6</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="Q21" s="11">
         <v>200</v>
       </c>
-      <c r="R21" s="10">
+      <c r="R21" s="12">
         <v>200</v>
       </c>
-      <c r="S21" s="11">
+      <c r="S21" s="15">
         <v>2900</v>
       </c>
-      <c r="T21" s="12">
+      <c r="T21" s="11">
         <f t="shared" si="0"/>
-        <v>8.9034699298143245</v>
-      </c>
-      <c r="U21" s="15">
+        <v>3.3929200658769769</v>
+      </c>
+      <c r="U21" s="14">
         <f t="shared" si="1"/>
-        <v>0.11231576092051274</v>
-      </c>
-      <c r="V21">
+        <v>0.18420711006006404</v>
+      </c>
+      <c r="V21" s="14">
         <v>0</v>
       </c>
-      <c r="W21" s="10">
+      <c r="W21" s="12">
         <f t="shared" si="12"/>
-        <v>449.26304368205098</v>
-      </c>
-      <c r="X21" s="16">
-        <v>0</v>
-      </c>
-      <c r="Y21">
+        <v>589.4627521922049</v>
+      </c>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14">
         <f t="shared" si="10"/>
-        <v>4000</v>
-      </c>
-      <c r="Z21" s="10">
+        <v>3200</v>
+      </c>
+      <c r="Z21" s="12">
         <f t="shared" si="11"/>
-        <v>4000</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="9">
-        <v>2.5</v>
-      </c>
+      <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="17">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>2000</v>
-      </c>
       <c r="K22" s="10"/>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="N22" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="O22" s="10">
-        <v>2</v>
-      </c>
-      <c r="P22" s="11">
-        <v>6</v>
-      </c>
-      <c r="Q22" s="9">
-        <v>200</v>
-      </c>
-      <c r="R22" s="10">
-        <v>200</v>
-      </c>
-      <c r="S22" s="11">
-        <v>2900</v>
-      </c>
+      <c r="M22" s="9"/>
+      <c r="O22" s="10"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="10"/>
       <c r="T22" s="9"/>
+      <c r="U22" s="14">
+        <f>(U17+U18+U19+U20+U21)/5</f>
+        <v>0.1228825634642589</v>
+      </c>
       <c r="W22" s="10"/>
       <c r="Z22" s="10"/>
     </row>
@@ -2901,19 +2878,6 @@
       <c r="T49" s="9"/>
       <c r="W49" s="10"/>
       <c r="Z49" s="10"/>
-    </row>
-    <row r="50" spans="3:26">
-      <c r="C50" s="9"/>
-      <c r="D50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="M50" s="9"/>
-      <c r="O50" s="10"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="10"/>
-      <c r="T50" s="9"/>
-      <c r="W50" s="10"/>
-      <c r="Z50" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>